<commit_message>
getting generic interface working again after NSMP specific work
</commit_message>
<xml_diff>
--- a/www/Configs/NSMP/Data Entry Template - NSMP.xlsx
+++ b/www/Configs/NSMP/Data Entry Template - NSMP.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/sea084_csiro_au/Documents/RossRCode/Git/Shiny/Apps/NationalSoilMonitoring/NSMData/www/Configs/NSMP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sea084\OneDrive - CSIRO\RossRCode\Git\Shiny\Apps\SoilDataEntry\www\Configs\NSMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1219" documentId="13_ncr:1_{806FB16B-895D-4BC9-A51C-3E69EFC0CC51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01CF15A1-2A9F-4270-B82D-84B83644B6C5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD645398-F41B-445B-9197-3D7D188121DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="-20910" windowWidth="25605" windowHeight="15495" firstSheet="1" activeTab="1" xr2:uid="{83C9EC8A-7EF8-4F9D-A138-3450D8759736}"/>
+    <workbookView xWindow="4425" yWindow="-16860" windowWidth="27855" windowHeight="17295" firstSheet="4" activeTab="4" xr2:uid="{83C9EC8A-7EF8-4F9D-A138-3450D8759736}"/>
   </bookViews>
   <sheets>
     <sheet name="TemplateOriginal" sheetId="1" state="hidden" r:id="rId1"/>
-    <sheet name="DBInfo" sheetId="8" r:id="rId2"/>
+    <sheet name="DBInfo" sheetId="8" state="hidden" r:id="rId2"/>
     <sheet name="DBTableLevels" sheetId="9" state="hidden" r:id="rId3"/>
-    <sheet name="Codes" sheetId="2" r:id="rId4"/>
+    <sheet name="Codes" sheetId="2" state="hidden" r:id="rId4"/>
     <sheet name="About" sheetId="13" r:id="rId5"/>
     <sheet name="Template" sheetId="4" r:id="rId6"/>
     <sheet name="Filled Example" sheetId="20" r:id="rId7"/>
@@ -9572,7 +9572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B47E6B88-97CE-436E-8F7D-17E89501757A}">
   <dimension ref="A1:AU33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="E4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="AQ4" sqref="AQ4"/>
     </sheetView>
   </sheetViews>
@@ -18951,7 +18951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064B206F-F17C-4025-942F-53FBF697F5D0}">
   <dimension ref="A1:AJ56"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -18982,6 +18982,16 @@
       <c r="X1" s="12"/>
       <c r="Y1" s="12"/>
       <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="12"/>
@@ -19010,6 +19020,16 @@
       <c r="X2" s="12"/>
       <c r="Y2" s="12"/>
       <c r="Z2" s="12"/>
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12"/>
+      <c r="AC2" s="12"/>
+      <c r="AD2" s="12"/>
+      <c r="AE2" s="12"/>
+      <c r="AF2" s="12"/>
+      <c r="AG2" s="12"/>
+      <c r="AH2" s="12"/>
+      <c r="AI2" s="12"/>
+      <c r="AJ2" s="12"/>
     </row>
     <row r="3" spans="1:36" ht="47.5" x14ac:dyDescent="1.1000000000000001">
       <c r="A3" s="12"/>
@@ -19040,6 +19060,16 @@
       <c r="X3" s="12"/>
       <c r="Y3" s="12"/>
       <c r="Z3" s="12"/>
+      <c r="AA3" s="12"/>
+      <c r="AB3" s="12"/>
+      <c r="AC3" s="12"/>
+      <c r="AD3" s="12"/>
+      <c r="AE3" s="12"/>
+      <c r="AF3" s="12"/>
+      <c r="AG3" s="12"/>
+      <c r="AH3" s="12"/>
+      <c r="AI3" s="12"/>
+      <c r="AJ3" s="12"/>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="12"/>
@@ -19068,6 +19098,16 @@
       <c r="X4" s="12"/>
       <c r="Y4" s="12"/>
       <c r="Z4" s="12"/>
+      <c r="AA4" s="12"/>
+      <c r="AB4" s="12"/>
+      <c r="AC4" s="12"/>
+      <c r="AD4" s="12"/>
+      <c r="AE4" s="12"/>
+      <c r="AF4" s="12"/>
+      <c r="AG4" s="12"/>
+      <c r="AH4" s="12"/>
+      <c r="AI4" s="12"/>
+      <c r="AJ4" s="12"/>
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" s="12"/>
@@ -19096,6 +19136,16 @@
       <c r="X5" s="12"/>
       <c r="Y5" s="12"/>
       <c r="Z5" s="12"/>
+      <c r="AA5" s="12"/>
+      <c r="AB5" s="12"/>
+      <c r="AC5" s="12"/>
+      <c r="AD5" s="12"/>
+      <c r="AE5" s="12"/>
+      <c r="AF5" s="12"/>
+      <c r="AG5" s="12"/>
+      <c r="AH5" s="12"/>
+      <c r="AI5" s="12"/>
+      <c r="AJ5" s="12"/>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" s="12"/>
@@ -19124,6 +19174,16 @@
       <c r="X6" s="12"/>
       <c r="Y6" s="12"/>
       <c r="Z6" s="12"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="12"/>
+      <c r="AC6" s="12"/>
+      <c r="AD6" s="12"/>
+      <c r="AE6" s="12"/>
+      <c r="AF6" s="12"/>
+      <c r="AG6" s="12"/>
+      <c r="AH6" s="12"/>
+      <c r="AI6" s="12"/>
+      <c r="AJ6" s="12"/>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" s="12"/>
@@ -19152,6 +19212,16 @@
       <c r="X7" s="12"/>
       <c r="Y7" s="12"/>
       <c r="Z7" s="12"/>
+      <c r="AA7" s="12"/>
+      <c r="AB7" s="12"/>
+      <c r="AC7" s="12"/>
+      <c r="AD7" s="12"/>
+      <c r="AE7" s="12"/>
+      <c r="AF7" s="12"/>
+      <c r="AG7" s="12"/>
+      <c r="AH7" s="12"/>
+      <c r="AI7" s="12"/>
+      <c r="AJ7" s="12"/>
     </row>
     <row r="8" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A8" s="12"/>
@@ -19182,6 +19252,16 @@
       <c r="X8" s="12"/>
       <c r="Y8" s="12"/>
       <c r="Z8" s="12"/>
+      <c r="AA8" s="12"/>
+      <c r="AB8" s="12"/>
+      <c r="AC8" s="12"/>
+      <c r="AD8" s="12"/>
+      <c r="AE8" s="12"/>
+      <c r="AF8" s="12"/>
+      <c r="AG8" s="12"/>
+      <c r="AH8" s="12"/>
+      <c r="AI8" s="12"/>
+      <c r="AJ8" s="12"/>
     </row>
     <row r="9" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A9" s="12"/>
@@ -19210,6 +19290,16 @@
       <c r="X9" s="12"/>
       <c r="Y9" s="12"/>
       <c r="Z9" s="12"/>
+      <c r="AA9" s="12"/>
+      <c r="AB9" s="12"/>
+      <c r="AC9" s="12"/>
+      <c r="AD9" s="12"/>
+      <c r="AE9" s="12"/>
+      <c r="AF9" s="12"/>
+      <c r="AG9" s="12"/>
+      <c r="AH9" s="12"/>
+      <c r="AI9" s="12"/>
+      <c r="AJ9" s="12"/>
     </row>
     <row r="10" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A10" s="12"/>
@@ -19240,6 +19330,16 @@
       <c r="X10" s="12"/>
       <c r="Y10" s="12"/>
       <c r="Z10" s="12"/>
+      <c r="AA10" s="12"/>
+      <c r="AB10" s="12"/>
+      <c r="AC10" s="12"/>
+      <c r="AD10" s="12"/>
+      <c r="AE10" s="12"/>
+      <c r="AF10" s="12"/>
+      <c r="AG10" s="12"/>
+      <c r="AH10" s="12"/>
+      <c r="AI10" s="12"/>
+      <c r="AJ10" s="12"/>
     </row>
     <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" s="12"/>
@@ -19268,6 +19368,16 @@
       <c r="X11" s="12"/>
       <c r="Y11" s="12"/>
       <c r="Z11" s="12"/>
+      <c r="AA11" s="12"/>
+      <c r="AB11" s="12"/>
+      <c r="AC11" s="12"/>
+      <c r="AD11" s="12"/>
+      <c r="AE11" s="12"/>
+      <c r="AF11" s="12"/>
+      <c r="AG11" s="12"/>
+      <c r="AH11" s="12"/>
+      <c r="AI11" s="12"/>
+      <c r="AJ11" s="12"/>
     </row>
     <row r="12" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A12" s="12"/>
@@ -19298,6 +19408,16 @@
       <c r="X12" s="12"/>
       <c r="Y12" s="12"/>
       <c r="Z12" s="12"/>
+      <c r="AA12" s="12"/>
+      <c r="AB12" s="12"/>
+      <c r="AC12" s="12"/>
+      <c r="AD12" s="12"/>
+      <c r="AE12" s="12"/>
+      <c r="AF12" s="12"/>
+      <c r="AG12" s="12"/>
+      <c r="AH12" s="12"/>
+      <c r="AI12" s="12"/>
+      <c r="AJ12" s="12"/>
     </row>
     <row r="13" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A13" s="12"/>
@@ -19328,6 +19448,16 @@
       <c r="X13" s="12"/>
       <c r="Y13" s="12"/>
       <c r="Z13" s="12"/>
+      <c r="AA13" s="12"/>
+      <c r="AB13" s="12"/>
+      <c r="AC13" s="12"/>
+      <c r="AD13" s="12"/>
+      <c r="AE13" s="12"/>
+      <c r="AF13" s="12"/>
+      <c r="AG13" s="12"/>
+      <c r="AH13" s="12"/>
+      <c r="AI13" s="12"/>
+      <c r="AJ13" s="12"/>
     </row>
     <row r="14" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A14" s="12"/>
@@ -19358,6 +19488,16 @@
       <c r="X14" s="12"/>
       <c r="Y14" s="12"/>
       <c r="Z14" s="12"/>
+      <c r="AA14" s="12"/>
+      <c r="AB14" s="12"/>
+      <c r="AC14" s="12"/>
+      <c r="AD14" s="12"/>
+      <c r="AE14" s="12"/>
+      <c r="AF14" s="12"/>
+      <c r="AG14" s="12"/>
+      <c r="AH14" s="12"/>
+      <c r="AI14" s="12"/>
+      <c r="AJ14" s="12"/>
     </row>
     <row r="15" spans="1:36" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A15" s="12"/>
@@ -20968,6 +21108,7 @@
       <c r="AJ56" s="12"/>
     </row>
   </sheetData>
+  <sheetProtection algorithmName="SHA-512" hashValue="yaq1X1OJqmdndO2v4B8tw9nPdbjHIx6UEYA+5RsEbCadPYKiPpi5NACsSM4HTvfIPuNTJqV1+SgEI0WtHfTixw==" saltValue="yl79cb33tVA6dZ4HUzdyQQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
various fixes for different dataset
</commit_message>
<xml_diff>
--- a/www/Configs/NSMP/Data Entry Template - NSMP.xlsx
+++ b/www/Configs/NSMP/Data Entry Template - NSMP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sea084\OneDrive - CSIRO\RossRCode\Git\Shiny\Apps\SoilDataEntry\www\Configs\NSMP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD645398-F41B-445B-9197-3D7D188121DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85FB1B30-9AB1-4C64-BF2C-F6282794E71A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4425" yWindow="-16860" windowWidth="27855" windowHeight="17295" firstSheet="4" activeTab="4" xr2:uid="{83C9EC8A-7EF8-4F9D-A138-3450D8759736}"/>
+    <workbookView xWindow="4400" yWindow="1680" windowWidth="18570" windowHeight="11530" firstSheet="4" activeTab="5" xr2:uid="{83C9EC8A-7EF8-4F9D-A138-3450D8759736}"/>
   </bookViews>
   <sheets>
     <sheet name="TemplateOriginal" sheetId="1" state="hidden" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2443" uniqueCount="1954">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2442" uniqueCount="1954">
   <si>
     <t>Site ID</t>
   </si>
@@ -18951,7 +18951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{064B206F-F17C-4025-942F-53FBF697F5D0}">
   <dimension ref="A1:AJ56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -21118,8 +21118,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A645384-9AAE-42FD-AF2D-5042FBACFF4E}">
   <dimension ref="A1:AU34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -21980,9 +21980,7 @@
       <c r="A14" s="2" t="s">
         <v>1532</v>
       </c>
-      <c r="B14" s="266" t="s">
-        <v>733</v>
-      </c>
+      <c r="B14" s="266"/>
       <c r="C14" s="112"/>
       <c r="D14" s="2" t="s">
         <v>1578</v>

</xml_diff>